<commit_message>
rewrite to include data driving login name and more conditional checks/recoveries
</commit_message>
<xml_diff>
--- a/ChangeSaaSPW/Default.xlsx
+++ b/ChangeSaaSPW/Default.xlsx
@@ -16,6 +16,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>ppm_octane@microfocus.com</t>
+  </si>
+  <si>
+    <t>j.kaplan@microfocus.com</t>
+  </si>
+  <si>
+    <t>c.ruth@microfocus.com</t>
+  </si>
+  <si>
+    <t>j.banks@microfocus.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -156,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,13 +184,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -469,16 +505,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row customFormat="1">
+      <c t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row>
+      <c s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed redundant tests; added browser check code to PW test
</commit_message>
<xml_diff>
--- a/ChangeSaaSPW/Default.xlsx
+++ b/ChangeSaaSPW/Default.xlsx
@@ -17,12 +17,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>userName</t>
   </si>
   <si>
     <t>ppm_octane@microfocus.com</t>
+  </si>
+  <si>
+    <t>a.madison@microfocus.com</t>
   </si>
   <si>
     <t>j.kaplan@microfocus.com</t>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -517,29 +520,34 @@
     <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1">
-      <c t="s">
+    <row r="1" ht="14.95" customFormat="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row>
-      <c s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row>
-      <c s="2" t="s">
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row>
-      <c s="2" t="s">
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row>
-      <c s="2" t="s">
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -560,7 +568,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -579,7 +587,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -598,7 +606,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed to use different initial password; and to use a fixed final password
</commit_message>
<xml_diff>
--- a/ChangeSaaSPW/Default.xlsx
+++ b/ChangeSaaSPW/Default.xlsx
@@ -28,13 +28,13 @@
     <t>a.madison@microfocus.com</t>
   </si>
   <si>
-    <t>j.kaplan@microfocus.com</t>
-  </si>
-  <si>
     <t>c.ruth@microfocus.com</t>
   </si>
   <si>
     <t>j.banks@microfocus.com</t>
+  </si>
+  <si>
+    <t>j.kaplan@microfocus.com</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -527,22 +527,22 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">

</xml_diff>